<commit_message>
done with duplicate roll and prn and logic for duplicate prn in database
</commit_message>
<xml_diff>
--- a/uploads/test2.xlsx
+++ b/uploads/test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FCAC469-5767-4A4B-94A0-CC0FB9F6CF4D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06673000-2EA2-4C27-962B-1243C60A71B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33C28D21-EA77-4E6C-AF8F-501FF34973E7}"/>
   </bookViews>
@@ -78,9 +78,6 @@
     <t xml:space="preserve">KOLHE PRANJAL MILIND </t>
   </si>
   <si>
-    <t>LAWATE  VISHAL  PRAKASH</t>
-  </si>
-  <si>
     <t>GAVATE SHUBHAM ANANDA</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>CHAVAN VAIBHAV BHOLENATH</t>
   </si>
   <si>
-    <t>PATHAK  VINAYAK VIJAY</t>
-  </si>
-  <si>
     <t>SONALKAR  PRANAV RAVINDRA</t>
   </si>
   <si>
@@ -274,12 +268,18 @@
   <si>
     <t>Shinde Vikram Avinash</t>
   </si>
+  <si>
+    <t>LAWATE VISHAL PRAKASH</t>
+  </si>
+  <si>
+    <t>PATHAK VINAYAK VIJAY</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +301,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -356,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -398,6 +404,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -715,7 +722,7 @@
   <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -868,8 +875,8 @@
       <c r="A11">
         <v>11</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>10</v>
+      <c r="B11" s="17" t="s">
+        <v>69</v>
       </c>
       <c r="C11" s="16">
         <v>2018032500121</v>
@@ -883,7 +890,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="16">
         <v>2018032500122</v>
@@ -897,7 +904,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="16">
         <v>2018032500123</v>
@@ -911,7 +918,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="16">
         <v>2018032500124</v>
@@ -925,7 +932,7 @@
         <v>15</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="16">
         <v>2018032500125</v>
@@ -939,7 +946,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="16">
         <v>2018032500126</v>
@@ -953,7 +960,7 @@
         <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="16">
         <v>2018032500127</v>
@@ -966,8 +973,8 @@
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>17</v>
+      <c r="B18" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="C18" s="16">
         <v>2018032500128</v>
@@ -981,7 +988,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C19" s="16">
         <v>2018032500129</v>
@@ -995,7 +1002,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C20" s="16">
         <v>2018032500130</v>
@@ -1009,7 +1016,7 @@
         <v>21</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C21" s="16">
         <v>2018032500131</v>
@@ -1023,7 +1030,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C22" s="16">
         <v>2018032500132</v>
@@ -1037,7 +1044,7 @@
         <v>23</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C23" s="16">
         <v>2018032500133</v>
@@ -1051,7 +1058,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C24" s="16">
         <v>2018032500134</v>
@@ -1065,7 +1072,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C25" s="16">
         <v>2018032500135</v>
@@ -1079,7 +1086,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C26" s="16">
         <v>2018032500136</v>
@@ -1093,7 +1100,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27" s="16">
         <v>2018032500137</v>
@@ -1107,7 +1114,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="16">
         <v>2018032500138</v>
@@ -1121,7 +1128,7 @@
         <v>29</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" s="16">
         <v>2018032500139</v>
@@ -1135,7 +1142,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C30" s="16">
         <v>2018032500140</v>
@@ -1149,7 +1156,7 @@
         <v>31</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C31" s="16">
         <v>2018032500141</v>
@@ -1163,7 +1170,7 @@
         <v>32</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C32" s="16">
         <v>2018032500142</v>
@@ -1177,7 +1184,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C33" s="16">
         <v>2018032500143</v>
@@ -1191,7 +1198,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C34" s="16">
         <v>2018032500144</v>
@@ -1205,7 +1212,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C35" s="16">
         <v>2018032500145</v>
@@ -1219,7 +1226,7 @@
         <v>36</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C36" s="16">
         <v>2018032500146</v>
@@ -1233,7 +1240,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C37" s="16">
         <v>2018032500147</v>
@@ -1247,7 +1254,7 @@
         <v>38</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" s="16">
         <v>2018032500148</v>
@@ -1261,7 +1268,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C39" s="16">
         <v>2018032500149</v>
@@ -1275,7 +1282,7 @@
         <v>40</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C40" s="16">
         <v>2018032500150</v>
@@ -1289,7 +1296,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C41" s="16">
         <v>2018032500151</v>
@@ -1303,7 +1310,7 @@
         <v>42</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C42" s="16">
         <v>2018032500152</v>
@@ -1317,7 +1324,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C43" s="16">
         <v>2018032500153</v>
@@ -1331,7 +1338,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C44" s="16">
         <v>2018032500154</v>
@@ -1345,7 +1352,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C45" s="16">
         <v>2018032500155</v>
@@ -1359,7 +1366,7 @@
         <v>46</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C46" s="16">
         <v>2018032500156</v>
@@ -1373,7 +1380,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C47" s="16">
         <v>2018032500157</v>
@@ -1387,7 +1394,7 @@
         <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C48" s="16">
         <v>2018032500158</v>
@@ -1401,7 +1408,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49" s="16">
         <v>2018032500159</v>
@@ -1415,7 +1422,7 @@
         <v>50</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C50" s="16">
         <v>2018032500160</v>
@@ -1429,7 +1436,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C51" s="16">
         <v>2018032500161</v>
@@ -1443,7 +1450,7 @@
         <v>52</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C52" s="16">
         <v>2018032500162</v>
@@ -1457,7 +1464,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C53" s="16">
         <v>2018032500163</v>
@@ -1471,7 +1478,7 @@
         <v>54</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C54" s="16">
         <v>2018032500164</v>
@@ -1485,7 +1492,7 @@
         <v>55</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C55" s="16">
         <v>2018032500165</v>
@@ -1499,7 +1506,7 @@
         <v>56</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C56" s="16">
         <v>2018032500166</v>
@@ -1513,7 +1520,7 @@
         <v>57</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C57" s="16">
         <v>2018032500167</v>
@@ -1527,7 +1534,7 @@
         <v>58</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C58" s="16">
         <v>2018032500168</v>
@@ -1541,7 +1548,7 @@
         <v>59</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C59" s="16">
         <v>2018032500169</v>
@@ -1555,7 +1562,7 @@
         <v>60</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C60" s="16">
         <v>2018032500170</v>
@@ -1569,7 +1576,7 @@
         <v>61</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C61" s="16">
         <v>2018032500171</v>
@@ -1583,7 +1590,7 @@
         <v>62</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C62" s="16">
         <v>2018032500172</v>
@@ -1597,7 +1604,7 @@
         <v>63</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C63" s="16">
         <v>2018032500173</v>
@@ -1611,7 +1618,7 @@
         <v>64</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C64" s="16">
         <v>2018032500174</v>
@@ -1625,7 +1632,7 @@
         <v>65</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C65" s="16">
         <v>2018032500175</v>
@@ -1636,7 +1643,7 @@
         <v>66</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C66" s="16">
         <v>2018032500176</v>
@@ -1647,7 +1654,7 @@
         <v>67</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C67" s="16">
         <v>2018032500177</v>
@@ -1658,7 +1665,7 @@
         <v>68</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C68" s="16">
         <v>2018032500178</v>
@@ -1669,7 +1676,7 @@
         <v>69</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C69" s="16">
         <v>2018032500179</v>
@@ -1680,7 +1687,7 @@
         <v>70</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C70" s="16">
         <v>2018032500180</v>
@@ -1691,7 +1698,7 @@
         <v>71</v>
       </c>
       <c r="B71" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C71" s="16">
         <v>2018032500181</v>

</xml_diff>